<commit_message>
Updated team theme rankings
</commit_message>
<xml_diff>
--- a/classes/1.30.19/theme-rankings-groupings.xlsx
+++ b/classes/1.30.19/theme-rankings-groupings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonayzman/Documents/Teaching/CSCI 499/Spring 2019/Administration/CSCI499/classes/1.30.19/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonayzman/Dropbox/Documents/Teaching/CSCI 499/Spring 2019/Administration/CSCI499/classes/1.30.19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF879A1D-3BC5-8C4D-B71E-8BDD0080AD68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A12E6CF-7524-5846-9A05-363D218CE518}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="460" windowWidth="23560" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23440" yWindow="6360" windowWidth="28040" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Groupings" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="44">
   <si>
     <t>Screen name</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Roy|12022141</t>
+  </si>
+  <si>
+    <t>Dropped</t>
   </si>
 </sst>
 </file>
@@ -667,7 +670,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -703,6 +706,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1058,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2503,6 +2507,11 @@
       </c>
       <c r="Q27" s="9">
         <v>43495.746759259258</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" s="29" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>